<commit_message>
adding AM and PM
</commit_message>
<xml_diff>
--- a/gCalROTC/formated_sheet.xlsx
+++ b/gCalROTC/formated_sheet.xlsx
@@ -49,7 +49,7 @@
     <t>2019/02/26</t>
   </si>
   <si>
-    <t>05:45</t>
+    <t>05:45 AM</t>
   </si>
   <si>
     <t>Personnel: BN Staff; UOD: NWUs/MARPATs; Execution Location: Battalion Spaces</t>
@@ -61,7 +61,7 @@
     <t>Muster/Quarters</t>
   </si>
   <si>
-    <t>06:10</t>
+    <t>06:10 AM</t>
   </si>
   <si>
     <t>Personnel: Battalion; UOD: NWUs/MARPATs; Execution Location: Gym Deck</t>
@@ -73,13 +73,13 @@
     <t>Formation</t>
   </si>
   <si>
-    <t>06:15</t>
+    <t>06:15 AM</t>
   </si>
   <si>
     <t>Pledge of Allegiance</t>
   </si>
   <si>
-    <t>06:20</t>
+    <t>06:20 AM</t>
   </si>
   <si>
     <t>Personnel: Battalion; UOD: NWUs/MARPATs; Execution Location: 202</t>
@@ -91,13 +91,13 @@
     <t>Announcements</t>
   </si>
   <si>
-    <t>06:22</t>
+    <t>06:22 AM</t>
   </si>
   <si>
     <t>Colorado Brief</t>
   </si>
   <si>
-    <t>06:25</t>
+    <t>06:25 AM</t>
   </si>
   <si>
     <t>Personnel: Battalion; UOD: NWUs/MARPATs; Execution Location: 202.0</t>
@@ -106,13 +106,13 @@
     <t>Head &amp; Water</t>
   </si>
   <si>
-    <t>06:35</t>
+    <t>06:35 AM</t>
   </si>
   <si>
     <t>ATFP</t>
   </si>
   <si>
-    <t>06:40</t>
+    <t>06:40 AM</t>
   </si>
   <si>
     <t>Personnel: Alpha Company; UOD: NWUs/MARPATs; Execution Location: Gym Deck</t>
@@ -130,25 +130,25 @@
     <t>Drill Showcase</t>
   </si>
   <si>
-    <t>07:50</t>
+    <t>07:50 AM</t>
   </si>
   <si>
     <t>CO's Remarks</t>
   </si>
   <si>
-    <t>08:25</t>
+    <t>08:25 AM</t>
   </si>
   <si>
     <t>Dismissed</t>
   </si>
   <si>
-    <t>08:35</t>
+    <t>08:35 AM</t>
   </si>
   <si>
     <t>Unit Staff Meeting</t>
   </si>
   <si>
-    <t>08:40</t>
+    <t>08:40 AM</t>
   </si>
   <si>
     <t>Personnel: BN Staff; UOD: NWUs/MARPATs; Execution Location: Main Office</t>
@@ -163,7 +163,7 @@
     <t>2019/02/27</t>
   </si>
   <si>
-    <t>05:30</t>
+    <t>05:30 AM</t>
   </si>
   <si>
     <t>Personnel: COD Team; UOD: BN PT Shirts; Execution Location: Gym Deck</t>
@@ -181,7 +181,7 @@
     <t>All Hands Field Day</t>
   </si>
   <si>
-    <t>07:30</t>
+    <t>07:30 AM</t>
   </si>
   <si>
     <t>Personnel: Battalion; UOD: BN PT Shirts; Execution Location: Armory</t>
@@ -193,7 +193,7 @@
     <t>Gen. Powell Leadership Academy Career Fair</t>
   </si>
   <si>
-    <t>12:30</t>
+    <t>12:30 AM</t>
   </si>
   <si>
     <t>Personnel: Volunteers; UOD: Khakis; Execution Location: Minehaha Center</t>
@@ -202,7 +202,7 @@
     <t>2019/02/28</t>
   </si>
   <si>
-    <t>06:00</t>
+    <t>06:00 AM</t>
   </si>
   <si>
     <t>Personnel: COD Team; UOD: Khakis; Execution Location: Fieldhouse</t>
@@ -211,7 +211,7 @@
     <t>Color Guard Practice</t>
   </si>
   <si>
-    <t>08:15</t>
+    <t>08:15 AM</t>
   </si>
   <si>
     <t>Personnel: Color Guard Team; UOD: NWUs/MARPATs; Execution Location: Gym Deck</t>
@@ -220,7 +220,7 @@
     <t>Depart for Colorado</t>
   </si>
   <si>
-    <t>18:45</t>
+    <t>6:45 PM</t>
   </si>
   <si>
     <t>Personnel: Drill Teams; UOD: PCA w/ Unit Polo; Execution Location: Gym Deck</t>
@@ -244,7 +244,7 @@
     <t>2019/03/03</t>
   </si>
   <si>
-    <t>22:00</t>
+    <t>10:00 PM</t>
   </si>
 </sst>
 </file>

</xml_diff>